<commit_message>
záloha 14.8.2023 - poslední návštěva terénu
</commit_message>
<xml_diff>
--- a/hodiny.xlsx
+++ b/hodiny.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabol\Desktop\Mapy\Bechyně 1-4000\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabol\Desktop\Mapy\Bechyne_1-4000\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E5498D2-086D-44AB-8D69-82978C557BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E09BA1-AB0C-43B1-A522-377FD52CA254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
   <si>
     <t>čas (h)</t>
   </si>
@@ -409,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:G29"/>
+  <dimension ref="C3:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -651,53 +651,92 @@
         <v>3</v>
       </c>
     </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C24" s="1">
+        <v>45151</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C25" s="1">
+        <v>45152</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25">
+        <v>112</v>
+      </c>
+    </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="1">
+        <v>45152</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C27" s="1"/>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C30" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D26">
+      <c r="D30">
         <v>250</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C27" s="3" t="s">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C31" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="2">
-        <f>SUM(D6:D25)</f>
-        <v>53.75</v>
-      </c>
-      <c r="E27" s="2" t="s">
+      <c r="D31" s="2">
+        <f>SUM(D6:D29)</f>
+        <v>61.75</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="D28" s="2">
-        <f>D26*D27</f>
-        <v>13437.5</v>
-      </c>
-      <c r="E28" s="2" t="s">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D32" s="2">
+        <f>D30*D31</f>
+        <v>15437.5</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C29" s="3" t="str">
+    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C33" s="3" t="str">
         <f>("+ náklady")</f>
         <v>+ náklady</v>
       </c>
-      <c r="D29" s="2">
-        <f>D28+SUM(F6:F25)+SUM(G6:G25)</f>
-        <v>14235.5</v>
-      </c>
-      <c r="E29" s="2" t="s">
+      <c r="D33" s="2">
+        <f>D32+SUM(F6:F29)+SUM(G6:G29)</f>
+        <v>16459.5</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="D27" formulaRange="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>